<commit_message>
switch all components to SMT
layout is a mess
</commit_message>
<xml_diff>
--- a/hardware/KiCad/nixieAccurateClock/daughter-board-placement.xlsx
+++ b/hardware/KiCad/nixieAccurateClock/daughter-board-placement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pwillis\Documents\GitHub\nixie-clock-ice\KiCad\nixieAccurateClock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\hardware\KiCad\nixieAccurateClock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5F6ACB6-05E1-4CCC-98DF-EFEBAD8FADE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE3924F-42B3-42B0-9FAE-21DF6B2A42C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="25580" windowHeight="15260" xr2:uid="{85BE6F36-083D-4018-98F1-367975EE3989}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{85BE6F36-083D-4018-98F1-367975EE3989}"/>
   </bookViews>
   <sheets>
     <sheet name="clock" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>width</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>width-mount</t>
+  </si>
+  <si>
+    <t>origin</t>
   </si>
 </sst>
 </file>
@@ -161,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -307,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,16 +460,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDA2DD0-EE20-45CA-901A-0F5B3918E4E1}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,16 +479,16 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <f>B13/2</f>
+        <f>B14/2</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -492,16 +497,16 @@
         <v>148.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <f>B14-B15+B13</f>
+        <f>B15-B16+B14</f>
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -509,7 +514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -518,7 +523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -527,7 +532,7 @@
         <v>52.400000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -536,7 +541,7 @@
         <v>10.48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -545,7 +550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -553,7 +558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -562,90 +567,98 @@
         <v>8.8000000000000025</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>15.875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
-        <v>11.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>6.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
-        <v>-0.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B16">
+        <v>-5.92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B18">
-        <f>B19+B$4+B$11</f>
-        <v>137.15000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B19">
+        <f>B20+B$4+B$11</f>
+        <v>158.19499999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>13</v>
       </c>
-      <c r="B19">
-        <f>B20+B$4+B$10</f>
-        <v>112.35000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="B20">
+        <f>B21+B$4+B$10</f>
+        <v>133.39499999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
         <v>14</v>
       </c>
-      <c r="B20">
-        <f>B21+B$4+B$11</f>
-        <v>83.350000000000009</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="B21">
+        <f>B22+B$4+B$11</f>
+        <v>104.395</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B21">
-        <f>B22+B$4+B$10</f>
-        <v>58.550000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B22">
+        <f>B23+B$4+B$10</f>
+        <v>79.594999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B22">
-        <f>B23+B$4+B$11</f>
-        <v>29.550000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B23">
+        <f>B24+B$4+B$11</f>
+        <v>50.595000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B23">
-        <f>B13-B15</f>
-        <v>4.75</v>
+      <c r="B24">
+        <f>B14-B16+B13</f>
+        <v>25.795000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -659,12 +672,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +685,7 @@
         <v>152.4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -681,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -690,7 +703,7 @@
         <v>148.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -699,7 +712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -707,7 +720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -716,7 +729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -725,7 +738,7 @@
         <v>52.400000000000006</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -734,7 +747,7 @@
         <v>10.48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -742,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -750,7 +763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -759,7 +772,7 @@
         <v>8.3500000000000014</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -767,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -775,7 +788,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -783,7 +796,7 @@
         <v>-0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -791,7 +804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -800,7 +813,7 @@
         <v>137.15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -809,7 +822,7 @@
         <v>112.80000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -818,7 +831,7 @@
         <v>88.45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -827,7 +840,7 @@
         <v>53.45</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -836,7 +849,7 @@
         <v>29.1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>17</v>
       </c>

</xml_diff>